<commit_message>
added some database documents
</commit_message>
<xml_diff>
--- a/database/IndexesTable.xlsx
+++ b/database/IndexesTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Query name</t>
   </si>
@@ -51,13 +51,16 @@
   </si>
   <si>
     <t>Difference (ms)</t>
+  </si>
+  <si>
+    <t>Percentage saved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +99,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -120,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -184,26 +195,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
     <cellStyle name="Total" xfId="4" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -482,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +526,7 @@
     <col min="5" max="5" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,8 +539,11 @@
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -525,8 +557,12 @@
         <f>B2-C2</f>
         <v>15</v>
       </c>
+      <c r="E2" s="5">
+        <f>(D2/B2)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -540,8 +576,12 @@
         <f t="shared" ref="D3:D6" si="0">B3-C3</f>
         <v>13</v>
       </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E6" si="1">(D3/B3)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -555,8 +595,12 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
+      <c r="E4" s="5">
+        <f t="shared" si="1"/>
+        <v>0.20454545454545456</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -570,8 +614,12 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
+      <c r="E5" s="5">
+        <f t="shared" si="1"/>
+        <v>7.7777777777777779E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -585,8 +633,12 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
+      <c r="E6" s="5">
+        <f t="shared" si="1"/>
+        <v>0.42857142857142855</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>